<commit_message>
[lab3] : fix comments
</commit_message>
<xml_diff>
--- a/lab3/measurements.xlsx
+++ b/lab3/measurements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Number of vessels</t>
-  </si>
-  <si>
-    <t>Time to reach consistency</t>
   </si>
   <si>
     <t>Lab2</t>
@@ -38,7 +35,7 @@
     <t>Lab3</t>
   </si>
   <si>
-    <t>The measurements were done by sending 15 add requests. I could not send more due Repy (Or Seattle restrictions)</t>
+    <t>The measurements were done by sending 12 add requests. I could not send more due Repy (Or Seattle restrictions)</t>
   </si>
 </sst>
 </file>
@@ -112,6 +109,1021 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Comparison between lab2 and lab3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lab2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feuil1!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lab3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feuil1!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$C$3:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2146610672"/>
+        <c:axId val="-2133000256"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2146610672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2133000256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2133000256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2146610672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A2:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -389,95 +1401,80 @@
     <col min="2" max="2" width="39.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>11.36</v>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1.42</v>
+      </c>
+      <c r="C4">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>3.31</v>
+      </c>
+      <c r="C5">
+        <v>1.65</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3.46</v>
+      </c>
+      <c r="C6">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>10.54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>10</v>
+      <c r="B7">
+        <v>3.64</v>
+      </c>
+      <c r="C7">
+        <v>3.78</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[lab3] : minor changes and workers for lab2
</commit_message>
<xml_diff>
--- a/lab3/measurements.xlsx
+++ b/lab3/measurements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -256,7 +256,7 @@
                   <c:v>3.46</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.64</c:v>
+                  <c:v>4.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -348,11 +348,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2146610672"/>
-        <c:axId val="-2133000256"/>
+        <c:axId val="-2135557184"/>
+        <c:axId val="-2136516928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2146610672"/>
+        <c:axId val="-2135557184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -395,7 +395,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133000256"/>
+        <c:crossAx val="-2136516928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -403,7 +403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133000256"/>
+        <c:axId val="-2136516928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -454,7 +454,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2146610672"/>
+        <c:crossAx val="-2135557184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1392,7 +1392,7 @@
   <dimension ref="A2:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1461,7 +1461,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>3.64</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C7">
         <v>3.78</v>

</xml_diff>